<commit_message>
all problem list-83 problems
</commit_message>
<xml_diff>
--- a/LeetCodeDB_all_problems.xlsx
+++ b/LeetCodeDB_all_problems.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="94">
   <si>
     <t>#</t>
   </si>
@@ -297,6 +297,15 @@
   </si>
   <si>
     <t>Number of Comments per Post </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>V1</t>
   </si>
 </sst>
 </file>
@@ -617,16 +626,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -642,8 +653,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>175</v>
       </c>
@@ -656,8 +670,11 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>176</v>
       </c>
@@ -670,8 +687,11 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>177</v>
       </c>
@@ -684,8 +704,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
@@ -699,7 +722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>180</v>
       </c>
@@ -713,7 +736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>181</v>
       </c>
@@ -727,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>182</v>
       </c>
@@ -741,7 +764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>183</v>
       </c>
@@ -755,7 +778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>184</v>
       </c>
@@ -769,7 +792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>185</v>
       </c>
@@ -783,7 +806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>196</v>
       </c>
@@ -797,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>197</v>
       </c>
@@ -811,7 +834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>262</v>
       </c>
@@ -825,7 +848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>511</v>
       </c>
@@ -839,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>512</v>
       </c>

</xml_diff>